<commit_message>
Clean up + added all statistic simulations.
</commit_message>
<xml_diff>
--- a/Documents/Conditions Statistics.xlsx
+++ b/Documents/Conditions Statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karol\Desktop\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Project\RPCDS\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3211B422-3916-4232-A67A-6271BD981904}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD5573C-7412-434D-9611-E21162EA804C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="5" xr2:uid="{D114E956-904F-4ACF-8D16-8AA9AC5ADDDF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{D114E956-904F-4ACF-8D16-8AA9AC5ADDDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Circulatory and Respiratory S&amp;S" sheetId="1" r:id="rId1"/>
@@ -803,7 +803,7 @@
             <c:numRef>
               <c:f>'Diabetes Type 1'!$E$4:$E$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1041,7 +1041,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -15778,8 +15778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784D8B56-4C2D-49FD-B88E-EECC9F539A7A}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15830,7 +15830,7 @@
         <f>ROUND($B$1*$B$14*B15*$F$14,0)</f>
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <f>D4/$B$1</f>
         <v>0</v>
       </c>
@@ -15851,7 +15851,7 @@
         <f t="shared" ref="D5:D12" si="2">ROUND($B$1*$B$14*B16*$F$14,0)</f>
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <f t="shared" ref="E5:E12" si="3">D5/$B$1</f>
         <v>1E-3</v>
       </c>
@@ -15872,7 +15872,7 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
@@ -15893,7 +15893,7 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <f t="shared" si="3"/>
         <v>2E-3</v>
       </c>
@@ -15914,7 +15914,7 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <f t="shared" si="3"/>
         <v>4.0000000000000001E-3</v>
       </c>
@@ -15935,7 +15935,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <f t="shared" si="3"/>
         <v>8.0000000000000002E-3</v>
       </c>
@@ -15956,7 +15956,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <f t="shared" si="3"/>
         <v>1.2E-2</v>
       </c>
@@ -15977,7 +15977,7 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <f t="shared" si="3"/>
         <v>1.0999999999999999E-2</v>
       </c>
@@ -15998,7 +15998,7 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <f t="shared" si="3"/>
         <v>6.0000000000000001E-3</v>
       </c>
@@ -16109,8 +16109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F8427-5CC5-4B70-B1DE-880C4CECCF51}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>